<commit_message>
cambios en la adicion
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Aplicaciones/Aplicaciones_puras/Resultados_Electricity_Final/Analisis/Ranking_Estadistico_HLN_DM.xlsx
+++ b/codigo_final_organizado/Aplicaciones/Aplicaciones_puras/Resultados_Electricity_Final/Analisis/Ranking_Estadistico_HLN_DM.xlsx
@@ -663,10 +663,10 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>2.303547128598697</v>
+        <v>2.360530197348857</v>
       </c>
       <c r="I7" t="n">
-        <v>1.42863055877776</v>
+        <v>1.507753183552359</v>
       </c>
     </row>
     <row r="8">
@@ -694,10 +694,10 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>2.73161819963037</v>
+        <v>2.742151682354039</v>
       </c>
       <c r="I8" t="n">
-        <v>1.833410085520729</v>
+        <v>1.791334535278701</v>
       </c>
     </row>
     <row r="9">
@@ -756,10 +756,10 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>4.397820476454382</v>
+        <v>3.061910308268288</v>
       </c>
       <c r="I10" t="n">
-        <v>3.794172854799224</v>
+        <v>1.904383464632066</v>
       </c>
     </row>
   </sheetData>
@@ -1222,16 +1222,16 @@
         <v>0.2011424336876124</v>
       </c>
       <c r="G2" t="n">
-        <v>0.05429819976152328</v>
+        <v>0.06546638157961904</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2100964211925602</v>
+        <v>0.2296290742447789</v>
       </c>
       <c r="I2" t="n">
         <v>0.298981196609335</v>
       </c>
       <c r="J2" t="n">
-        <v>0.243366415763135</v>
+        <v>0.4370194909566052</v>
       </c>
     </row>
     <row r="3">
@@ -1256,16 +1256,16 @@
         <v>0.7457256578307847</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3040323196039247</v>
+        <v>0.3196842051293389</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3785311530338078</v>
+        <v>0.3611971997491434</v>
       </c>
       <c r="I3" t="n">
         <v>0.8129217329015264</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2438930796004684</v>
+        <v>0.8714115499384436</v>
       </c>
     </row>
     <row r="4">
@@ -1290,16 +1290,16 @@
         <v>0.817263123910557</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2897378152196299</v>
+        <v>0.3010811264265782</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3358213246504107</v>
+        <v>0.3308286524259445</v>
       </c>
       <c r="I4" t="n">
         <v>0.5488730847793386</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5915414588093793</v>
+        <v>0.53251175688164</v>
       </c>
     </row>
     <row r="5">
@@ -1324,16 +1324,16 @@
         <v>0.9693497243470433</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1730128379353029</v>
+        <v>0.1927496505398922</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3613269650562381</v>
+        <v>0.3733633158884433</v>
       </c>
       <c r="I5" t="n">
         <v>0.4932688773726057</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1255802009837059</v>
+        <v>0.5675821404899604</v>
       </c>
     </row>
     <row r="6">
@@ -1358,16 +1358,16 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.09877083499468209</v>
+        <v>0.1151776154665982</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2976817585769744</v>
+        <v>0.3178144093142117</v>
       </c>
       <c r="I6" t="n">
         <v>0.4517167789503451</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2299447194113031</v>
+        <v>0.5769710716092553</v>
       </c>
     </row>
     <row r="7">
@@ -1377,31 +1377,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.05429819976152328</v>
+        <v>0.06546638157961904</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3040323196039247</v>
+        <v>0.3196842051293389</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2897378152196299</v>
+        <v>0.3010811264265782</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1730128379353029</v>
+        <v>0.1927496505398922</v>
       </c>
       <c r="F7" t="n">
-        <v>0.09877083499468209</v>
+        <v>0.1151776154665982</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2325071556039897</v>
+        <v>0.2890165462237508</v>
       </c>
       <c r="I7" t="n">
-        <v>0.05389665253188847</v>
+        <v>0.07858805481375941</v>
       </c>
       <c r="J7" t="n">
-        <v>0.008734258113705984</v>
+        <v>0.117579344021491</v>
       </c>
     </row>
     <row r="8">
@@ -1411,31 +1411,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2100964211925602</v>
+        <v>0.2296290742447789</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3785311530338078</v>
+        <v>0.3611971997491434</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3358213246504107</v>
+        <v>0.3308286524259445</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3613269650562381</v>
+        <v>0.3733633158884433</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2976817585769744</v>
+        <v>0.3178144093142117</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2325071556039897</v>
+        <v>0.2890165462237508</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.4716399104781648</v>
+        <v>0.5213751693337416</v>
       </c>
       <c r="J8" t="n">
-        <v>0.03939073589374265</v>
+        <v>0.208987530822311</v>
       </c>
     </row>
     <row r="9">
@@ -1460,16 +1460,16 @@
         <v>0.4517167789503451</v>
       </c>
       <c r="G9" t="n">
-        <v>0.05389665253188847</v>
+        <v>0.07858805481375941</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4716399104781648</v>
+        <v>0.5213751693337416</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.004958155417663646</v>
+        <v>0.7166267432886311</v>
       </c>
     </row>
     <row r="10">
@@ -1479,28 +1479,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.243366415763135</v>
+        <v>0.4370194909566052</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2438930796004684</v>
+        <v>0.8714115499384436</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5915414588093793</v>
+        <v>0.53251175688164</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1255802009837059</v>
+        <v>0.5675821404899604</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2299447194113031</v>
+        <v>0.5769710716092553</v>
       </c>
       <c r="G10" t="n">
-        <v>0.008734258113705984</v>
+        <v>0.117579344021491</v>
       </c>
       <c r="H10" t="n">
-        <v>0.03939073589374265</v>
+        <v>0.208987530822311</v>
       </c>
       <c r="I10" t="n">
-        <v>0.004958155417663646</v>
+        <v>0.7166267432886311</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -1594,16 +1594,16 @@
         <v>1.52838221439589</v>
       </c>
       <c r="G2" t="n">
-        <v>2.696369642333581</v>
+        <v>2.518427412732279</v>
       </c>
       <c r="H2" t="n">
-        <v>1.491512981976511</v>
+        <v>1.416312553198512</v>
       </c>
       <c r="I2" t="n">
         <v>1.192468076339017</v>
       </c>
       <c r="J2" t="n">
-        <v>-1.367159680089101</v>
+        <v>0.8625711600869045</v>
       </c>
     </row>
     <row r="3">
@@ -1628,16 +1628,16 @@
         <v>-0.347506756476778</v>
       </c>
       <c r="G3" t="n">
-        <v>1.178173861933883</v>
+        <v>1.13524266567742</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9892728131653153</v>
+        <v>1.030039409186893</v>
       </c>
       <c r="I3" t="n">
         <v>0.2527458864954139</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.365330345710413</v>
+        <v>0.1725125760959997</v>
       </c>
     </row>
     <row r="4">
@@ -1662,16 +1662,16 @@
         <v>0.2467290701881985</v>
       </c>
       <c r="G4" t="n">
-        <v>1.219223381219321</v>
+        <v>1.186498229823468</v>
       </c>
       <c r="H4" t="n">
-        <v>1.092958718225459</v>
+        <v>1.105839399979577</v>
       </c>
       <c r="I4" t="n">
         <v>0.6538820586585872</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.5824089572267351</v>
+        <v>0.682301827240309</v>
       </c>
     </row>
     <row r="5">
@@ -1696,16 +1696,16 @@
         <v>-0.04088126211567304</v>
       </c>
       <c r="G5" t="n">
-        <v>1.656248482402415</v>
+        <v>1.564495524416255</v>
       </c>
       <c r="H5" t="n">
-        <v>1.029727903965078</v>
+        <v>1.001253100487087</v>
       </c>
       <c r="I5" t="n">
         <v>0.7531360695554763</v>
       </c>
       <c r="J5" t="n">
-        <v>-1.93162700273884</v>
+        <v>0.6220977151477445</v>
       </c>
     </row>
     <row r="6">
@@ -1730,16 +1730,16 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>2.142852736678887</v>
+        <v>2.00711321810901</v>
       </c>
       <c r="H6" t="n">
-        <v>1.19618194118757</v>
+        <v>1.140267738152051</v>
       </c>
       <c r="I6" t="n">
         <v>0.8329514642842605</v>
       </c>
       <c r="J6" t="n">
-        <v>-1.415150721765756</v>
+        <v>0.6064148509362324</v>
       </c>
     </row>
     <row r="7">
@@ -1749,31 +1749,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-2.696369642333581</v>
+        <v>-2.518427412732279</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.178173861933883</v>
+        <v>-1.13524266567742</v>
       </c>
       <c r="D7" t="n">
-        <v>-1.219223381219321</v>
+        <v>-1.186498229823468</v>
       </c>
       <c r="E7" t="n">
-        <v>-1.656248482402415</v>
+        <v>-1.564495524416255</v>
       </c>
       <c r="F7" t="n">
-        <v>-2.142852736678887</v>
+        <v>-2.00711321810901</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.405777261838097</v>
+        <v>-1.221344854142138</v>
       </c>
       <c r="I7" t="n">
-        <v>-2.703534936458579</v>
+        <v>-2.349152721356929</v>
       </c>
       <c r="J7" t="n">
-        <v>-4.786441897636824</v>
+        <v>-1.989042107580228</v>
       </c>
     </row>
     <row r="8">
@@ -1783,31 +1783,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-1.491512981976511</v>
+        <v>-1.416312553198512</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.9892728131653153</v>
+        <v>-1.030039409186893</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.092958718225459</v>
+        <v>-1.105839399979577</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.029727903965078</v>
+        <v>-1.001253100487087</v>
       </c>
       <c r="F8" t="n">
-        <v>-1.19618194118757</v>
+        <v>-1.140267738152051</v>
       </c>
       <c r="G8" t="n">
-        <v>1.405777261838097</v>
+        <v>1.221344854142138</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.7940005710509913</v>
+        <v>-0.7020039879691905</v>
       </c>
       <c r="J8" t="n">
-        <v>-3.014109446096883</v>
+        <v>-1.495991381269842</v>
       </c>
     </row>
     <row r="9">
@@ -1832,16 +1832,16 @@
         <v>-0.8329514642842605</v>
       </c>
       <c r="G9" t="n">
-        <v>2.703534936458579</v>
+        <v>2.349152721356929</v>
       </c>
       <c r="H9" t="n">
-        <v>0.7940005710509913</v>
+        <v>0.7020039879691905</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>-5.610573234619653</v>
+        <v>-0.3896871931125849</v>
       </c>
     </row>
     <row r="10">
@@ -1851,28 +1851,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.367159680089101</v>
+        <v>-0.8625711600869045</v>
       </c>
       <c r="C10" t="n">
-        <v>1.365330345710413</v>
+        <v>-0.1725125760959997</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5824089572267351</v>
+        <v>-0.682301827240309</v>
       </c>
       <c r="E10" t="n">
-        <v>1.93162700273884</v>
+        <v>-0.6220977151477445</v>
       </c>
       <c r="F10" t="n">
-        <v>1.415150721765756</v>
+        <v>-0.6064148509362324</v>
       </c>
       <c r="G10" t="n">
-        <v>4.786441897636824</v>
+        <v>1.989042107580228</v>
       </c>
       <c r="H10" t="n">
-        <v>3.014109446096883</v>
+        <v>1.495991381269842</v>
       </c>
       <c r="I10" t="n">
-        <v>5.610573234619653</v>
+        <v>0.3896871931125849</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>

</xml_diff>